<commit_message>
Signed-off-by: Sarowar Alam Saidi <sarowaralam47@gmail.com>
</commit_message>
<xml_diff>
--- a/testxlfile.xlsx
+++ b/testxlfile.xlsx
@@ -671,8 +671,16 @@
           <t>Tuesday</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n"/>
-      <c r="C2" s="2" t="n"/>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>tuesday pronunciation american</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>tuesday</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -680,8 +688,16 @@
           <t>Baby</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n"/>
-      <c r="C3" s="2" t="n"/>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>baby pink color</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Baby</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n"/>

</xml_diff>